<commit_message>
Deploying to main from @ INTI-CMNB/kibot_variants_arduprog@b1395b06b775338f18fba7b6877c7e3b8e0ab86a 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/t1-bom.xlsx
+++ b/BoM/Costs/t1-bom.xlsx
@@ -1281,7 +1281,7 @@
     <t>R_0805_2012Metric</t>
   </si>
   <si>
-    <t>http://search.murata.co.jp/Ceramy/image/img/PDF/ENG/L0110S0100BLM21P.pdf</t>
+    <t>https://www.murata.com/en-eu/api/pdfdownloadapi?cate=cgsubChipFerriBead&amp;partno=BLM21PG221SN1%23</t>
   </si>
   <si>
     <t>Murata</t>
@@ -1644,7 +1644,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>6.0.5+dfsg-1~bpo11+1</t>
+    <t>6.0.7+dfsg-1~bpo11+1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -1737,10 +1737,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2022-06-14 18:11:51</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.9 + KiBot v1.1.0</t>
+    <t>2022-09-27 14:31:50</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.13 + KiBot v1.3.0</t>
   </si>
   <si>
     <t>KiCad Fields (default)</t>

</xml_diff>

<commit_message>
Deploying to main from @ INTI-CMNB/kibot_variants_arduprog@3cac4a30831aabb85f0106ca408806fa45884664 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/t1-bom.xlsx
+++ b/BoM/Costs/t1-bom.xlsx
@@ -1737,10 +1737,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2022-09-27 14:31:50</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.13 + KiBot v1.3.0</t>
+    <t>2022-09-27 14:39:57</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.12 + KiBot v1.3.0</t>
   </si>
   <si>
     <t>KiCad Fields (default)</t>

</xml_diff>

<commit_message>
Deploying to main from @ INTI-CMNB/kibot_variants_arduprog@a8d83a141a3a344018021119b3d3ad7fe614f956 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/t1-bom.xlsx
+++ b/BoM/Costs/t1-bom.xlsx
@@ -1644,7 +1644,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>6.0.7+dfsg-1~bpo11+1</t>
+    <t>6.0.8+dfsg-1~bpo11+1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -1737,10 +1737,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2022-09-27 16:49:35</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.12 + KiBot v1.3.0</t>
+    <t>2022-10-21 15:26:27</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.13 + KiBot v1.4.0</t>
   </si>
   <si>
     <t>KiCad Fields (default)</t>

</xml_diff>

<commit_message>
Deploying to main from @ INTI-CMNB/kibot_variants_arduprog@d2b24e85d25f410070998b779f0c8304e9a05ba4 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/t1-bom.xlsx
+++ b/BoM/Costs/t1-bom.xlsx
@@ -1737,10 +1737,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2022-10-21 17:03:32</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.13 + KiBot v1.4.0</t>
+    <t>2022-10-21 17:28:11</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.13 + KiBot v1.4.1</t>
   </si>
   <si>
     <t>KiCad Fields (default)</t>

</xml_diff>

<commit_message>
Deploying to main from @ set-soft/kibot_variants_arduprog_test@ca7a833f839fabc32aedfdd6f0e9e60ef78d4d4a 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/t1-bom.xlsx
+++ b/BoM/Costs/t1-bom.xlsx
@@ -1644,7 +1644,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>6.0.8+dfsg-1~bpo11+1</t>
+    <t>6.0.9+dfsg-1~bpo11+1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -1737,10 +1737,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2022-10-21 17:47:18</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.12 + KiBot v1.4.0</t>
+    <t>2022-12-02 15:33:33</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.13 + KiBot v1.4.1</t>
   </si>
   <si>
     <t>KiCad Fields (default)</t>

</xml_diff>

<commit_message>
Deploying to main from @ set-soft/kibot_variants_arduprog_test@cb758b3d1ea9081fcbefeaa1248e2bda74c6af8d 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/t1-bom.xlsx
+++ b/BoM/Costs/t1-bom.xlsx
@@ -1737,10 +1737,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2022-12-16 11:24:48</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.15 + KiBot v1.4.1</t>
+    <t>2022-12-16 16:00:35</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.15 + KiBot v1.5.1</t>
   </si>
   <si>
     <t>KiCad Fields (default)</t>

</xml_diff>

<commit_message>
Deploying to main from @ set-soft/kibot_variants_arduprog_test@d26131a165992d108604e1ce75c4e528e1a92e71 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/t1-bom.xlsx
+++ b/BoM/Costs/t1-bom.xlsx
@@ -1644,7 +1644,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>6.0.9+dfsg-1~bpo11+1</t>
+    <t>6.0.10+dfsg-1~bpo11+1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -1737,7 +1737,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2022-12-16 16:00:35</t>
+    <t>2023-01-20 02:53:48</t>
   </si>
   <si>
     <t>KiCost® v1.1.15 + KiBot v1.5.1</t>
@@ -3821,7 +3821,7 @@
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="47.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="61.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="22.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" customWidth="1" outlineLevel="1"/>

</xml_diff>

<commit_message>
Deploying to main from @ set-soft/kibot_variants_arduprog_test@8834c161ae07edff2ac39e52a773db67d820afd8 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/t1-bom.xlsx
+++ b/BoM/Costs/t1-bom.xlsx
@@ -776,10 +776,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-01-20 18:49:04</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.15 + KiBot v1.5.2</t>
+    <t>2023-02-06 16:55:22</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.15 + KiBot v1.6.1</t>
   </si>
   <si>
     <t>KiCad Fields (default)</t>

</xml_diff>

<commit_message>
Deploying to main from @ set-soft/kibot_variants_arduprog_test@5586ec87a2bf3e38593cc15f910f4f380cdd90ea 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/t1-bom.xlsx
+++ b/BoM/Costs/t1-bom.xlsx
@@ -575,7 +575,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>6.0.10+dfsg-1~bpo11+1</t>
+    <t>6.0.11+dfsg-1~bpo11+1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -776,10 +776,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2023-02-06 16:55:22</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.15 + KiBot v1.6.1</t>
+    <t>2023-06-13 14:12:28</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.17 + KiBot v1.6.3</t>
   </si>
   <si>
     <t>KiCad Fields (default)</t>
@@ -840,12 +840,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -937,6 +931,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="19">
@@ -1061,19 +1061,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1100,22 +1099,22 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1124,26 +1123,26 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1165,7 +1164,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -1180,7 +1179,16 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="logo.png"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1208,7 +1216,7 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -1223,7 +1231,16 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="logo.png"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1251,7 +1268,7 @@
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -1266,7 +1283,16 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="logo.png"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1294,7 +1320,7 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -1309,7 +1335,16 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="logo.png"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1644,580 +1679,580 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="L9" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="13" t="s">
+      <c r="K10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="K11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="L11" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="13" t="s">
+      <c r="K12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="L12" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="30.0" customHeight="1">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:12" ht="30" customHeight="1">
+      <c r="A13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="J13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="K13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L13" s="7" t="s">
+      <c r="L13" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="J14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="K14" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="L14" s="11" t="s">
+      <c r="L14" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="45.0" customHeight="1">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:12" ht="45" customHeight="1">
+      <c r="A15" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="J15" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="K15" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="L15" s="7" t="s">
+      <c r="L15" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="30.0" customHeight="1">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:12" ht="30" customHeight="1">
+      <c r="A16" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="13" t="s">
+      <c r="K16" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="13" t="s">
+      <c r="L16" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="30.0" customHeight="1">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:12" ht="30" customHeight="1">
+      <c r="A17" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="9" t="s">
+      <c r="J17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K17" s="9" t="s">
+      <c r="K17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L17" s="9" t="s">
+      <c r="L17" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="I18" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="13" t="s">
+      <c r="J18" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="K18" s="13" t="s">
+      <c r="K18" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="L18" s="13" t="s">
+      <c r="L18" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I19" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="9" t="s">
+      <c r="J19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K19" s="9" t="s">
+      <c r="K19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L19" s="9" t="s">
+      <c r="L19" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="12" t="s">
+      <c r="I20" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="J20" s="13" t="s">
+      <c r="J20" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="K20" s="13" t="s">
+      <c r="K20" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="L20" s="13" t="s">
+      <c r="L20" s="12" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2257,466 +2292,466 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="L9" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="K10" s="13" t="s">
+      <c r="K10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30.0" customHeight="1">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:12" ht="30" customHeight="1">
+      <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="K11" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="L11" s="6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="45.0" customHeight="1">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:12" ht="45" customHeight="1">
+      <c r="A12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="J12" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="L12" s="11" t="s">
+      <c r="L12" s="10" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="45.0" customHeight="1">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:12" ht="45" customHeight="1">
+      <c r="A13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="J13" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="K13" s="7" t="s">
+      <c r="K13" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="L13" s="7" t="s">
+      <c r="L13" s="6" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="11" t="s">
+      <c r="J14" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="K14" s="13" t="s">
+      <c r="K14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="L14" s="13" t="s">
+      <c r="L14" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="J15" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="9" t="s">
+      <c r="L15" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="J16" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="K16" s="11" t="s">
+      <c r="K16" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="L16" s="11" t="s">
+      <c r="L16" s="10" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="J17" s="7" t="s">
+      <c r="J17" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="K17" s="7" t="s">
+      <c r="K17" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="L17" s="7" t="s">
+      <c r="L17" s="6" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2753,360 +2788,360 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="16">
         <f>SUM(G10:G21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="18" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="19">
         <f>CEILING(BoardQty*4,1)</f>
         <v>4</v>
       </c>
-      <c r="G10" s="21" t="str">
+      <c r="G10" s="20">
         <f>IF(AND(ISNUMBER(E10),ISNUMBER(F10)),E10*F10,"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G11" s="21" t="str">
+      <c r="G11" s="20">
         <f>IF(AND(ISNUMBER(E11),ISNUMBER(F11)),E11*F11,"")</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G12" s="21" t="str">
+      <c r="G12" s="20">
         <f>IF(AND(ISNUMBER(E12),ISNUMBER(F12)),E12*F12,"")</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G13" s="21" t="str">
+      <c r="G13" s="20">
         <f>IF(AND(ISNUMBER(E13),ISNUMBER(F13)),E13*F13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30.0" customHeight="1">
-      <c r="A14" s="20" t="s">
+    <row r="14" spans="1:7" ht="30" customHeight="1">
+      <c r="A14" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="19">
         <f>CEILING(BoardQty*2,1)</f>
         <v>2</v>
       </c>
-      <c r="G14" s="21" t="str">
+      <c r="G14" s="20">
         <f>IF(AND(ISNUMBER(E14),ISNUMBER(F14)),E14*F14,"")</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G15" s="21" t="str">
+      <c r="G15" s="20">
         <f>IF(AND(ISNUMBER(E15),ISNUMBER(F15)),E15*F15,"")</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G16" s="21" t="str">
+      <c r="G16" s="20">
         <f>IF(AND(ISNUMBER(E16),ISNUMBER(F16)),E16*F16,"")</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G17" s="21" t="str">
+      <c r="G17" s="20">
         <f>IF(AND(ISNUMBER(E17),ISNUMBER(F17)),E17*F17,"")</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G18" s="21" t="str">
+      <c r="G18" s="20">
         <f>IF(AND(ISNUMBER(E18),ISNUMBER(F18)),E18*F18,"")</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="20">
+      <c r="E19" s="19">
         <f>CEILING(BoardQty*3,1)</f>
         <v>3</v>
       </c>
-      <c r="G19" s="21" t="str">
+      <c r="G19" s="20">
         <f>IF(AND(ISNUMBER(E19),ISNUMBER(F19)),E19*F19,"")</f>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E20" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G20" s="21" t="str">
+      <c r="G20" s="20">
         <f>IF(AND(ISNUMBER(E20),ISNUMBER(F20)),E20*F20,"")</f>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E21" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G21" s="21" t="str">
+      <c r="G21" s="20">
         <f>IF(AND(ISNUMBER(E21),ISNUMBER(F21)),E21*F21,"")</f>
         <v/>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="22" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="23" t="s">
         <v>171</v>
       </c>
     </row>
@@ -3211,306 +3246,306 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="16">
         <f>SUM(G10:G18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="18" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
         <v>2</v>
       </c>
-      <c r="G10" s="21" t="str">
+      <c r="G10" s="20">
         <f>IF(AND(ISNUMBER(E10),ISNUMBER(F10)),E10*F10,"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G11" s="21" t="str">
+      <c r="G11" s="20">
         <f>IF(AND(ISNUMBER(E11),ISNUMBER(F11)),E11*F11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30.0" customHeight="1">
-      <c r="A12" s="20" t="s">
+    <row r="12" spans="1:7" ht="30" customHeight="1">
+      <c r="A12" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G12" s="21" t="str">
+      <c r="G12" s="20">
         <f>IF(AND(ISNUMBER(E12),ISNUMBER(F12)),E12*F12,"")</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G13" s="21" t="str">
+      <c r="G13" s="20">
         <f>IF(AND(ISNUMBER(E13),ISNUMBER(F13)),E13*F13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45.0" customHeight="1">
-      <c r="A14" s="20" t="s">
+    <row r="14" spans="1:7" ht="45" customHeight="1">
+      <c r="A14" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G14" s="21" t="str">
+      <c r="G14" s="20">
         <f>IF(AND(ISNUMBER(E14),ISNUMBER(F14)),E14*F14,"")</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
         <v>2</v>
       </c>
-      <c r="G15" s="21" t="str">
+      <c r="G15" s="20">
         <f>IF(AND(ISNUMBER(E15),ISNUMBER(F15)),E15*F15,"")</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G16" s="21" t="str">
+      <c r="G16" s="20">
         <f>IF(AND(ISNUMBER(E16),ISNUMBER(F16)),E16*F16,"")</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="19">
         <f>CEILING(BoardQty*2,1)</f>
         <v>2</v>
       </c>
-      <c r="G17" s="21" t="str">
+      <c r="G17" s="20">
         <f>IF(AND(ISNUMBER(E17),ISNUMBER(F17)),E17*F17,"")</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G18" s="21" t="str">
+      <c r="G18" s="20">
         <f>IF(AND(ISNUMBER(E18),ISNUMBER(F18)),E18*F18,"")</f>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="22" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="23" t="s">
         <v>171</v>
       </c>
     </row>
@@ -3590,22 +3625,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3615,47 +3650,47 @@
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="26" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="28" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="29" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="30" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="31" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="32" t="s">
         <v>185</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deploying to main from @ set-soft/kibot_variants_arduprog_test@4c902ffc0bfb5f10c674151ab507c1e9b408fded 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/t1-bom.xlsx
+++ b/BoM/Costs/t1-bom.xlsx
@@ -575,7 +575,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>6.0.11+dfsg-1</t>
+    <t>7.0.9-7.0.9~ubuntu23.04.1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -776,7 +776,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-02-01 12:19:07</t>
+    <t>2024-02-01 13:50:25</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.4</t>
@@ -1667,7 +1667,7 @@
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="23.7109375" customWidth="1"/>
     <col min="6" max="6" width="46.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
@@ -2280,7 +2280,7 @@
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="44.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
@@ -2782,7 +2782,7 @@
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="42.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="60.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
   </cols>
@@ -3240,7 +3240,7 @@
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="40.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="61.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Deploying to main from @ set-soft/kibot_variants_arduprog_test@59bc16bcb8045deef2bec1276978eb984cf0d225 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/t1-bom.xlsx
+++ b/BoM/Costs/t1-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="170">
   <si>
     <t>Row</t>
   </si>
@@ -305,7 +305,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>Unpolarized capacitor</t>
+    <t/>
   </si>
   <si>
     <t>C</t>
@@ -329,9 +329,6 @@
     <t>~</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -344,9 +341,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>Polarized capacitor</t>
-  </si>
-  <si>
     <t>C_Polarized</t>
   </si>
   <si>
@@ -368,9 +362,6 @@
     <t>MAL215371479E3</t>
   </si>
   <si>
-    <t>Diode</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -386,9 +377,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>Light emitting diode</t>
-  </si>
-  <si>
     <t>LED</t>
   </si>
   <si>
@@ -410,9 +398,6 @@
     <t>6</t>
   </si>
   <si>
-    <t>DC Barrel Jack with an internal switch</t>
-  </si>
-  <si>
     <t>Barrel_Jack_Switch</t>
   </si>
   <si>
@@ -434,9 +419,6 @@
     <t>7</t>
   </si>
   <si>
-    <t>Generic connector, double row, 02x03, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
     <t>Conn_02x03_Odd_Even</t>
   </si>
   <si>
@@ -464,9 +446,6 @@
     <t>8</t>
   </si>
   <si>
-    <t>Generic connector, single row, 01x05, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
     <t>Conn_01x05_Male</t>
   </si>
   <si>
@@ -482,9 +461,6 @@
     <t>9</t>
   </si>
   <si>
-    <t>Generic connector, single row, 01x06, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
     <t>Conn_01x06_Male</t>
   </si>
   <si>
@@ -500,9 +476,6 @@
     <t>10</t>
   </si>
   <si>
-    <t>Resistor</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -527,9 +500,6 @@
     <t>12</t>
   </si>
   <si>
-    <t>16MHz, 8kB Flash, 512B SRAM, 512B EEPROM, TQFP-32</t>
-  </si>
-  <si>
     <t>ATmega8U2-A</t>
   </si>
   <si>
@@ -575,7 +545,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>7.0.9-7.0.9~ubuntu23.04.1</t>
+    <t>8.0.1+dfsg-1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -611,9 +581,6 @@
     <t>+USB,+XTAL</t>
   </si>
   <si>
-    <t>Resettable fuse, polymeric positive temperature coefficient</t>
-  </si>
-  <si>
     <t>Polyfuse</t>
   </si>
   <si>
@@ -632,9 +599,6 @@
     <t>+USB</t>
   </si>
   <si>
-    <t>Ferrite bead</t>
-  </si>
-  <si>
     <t>FerriteBead</t>
   </si>
   <si>
@@ -650,9 +614,6 @@
     <t>Murata</t>
   </si>
   <si>
-    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
-  </si>
-  <si>
     <t>Conn_02x02_Odd_Even</t>
   </si>
   <si>
@@ -671,9 +632,6 @@
     <t>M20-9980246-ND</t>
   </si>
   <si>
-    <t>USB Type B connector</t>
-  </si>
-  <si>
     <t>USB_B</t>
   </si>
   <si>
@@ -704,9 +662,6 @@
     <t>1M</t>
   </si>
   <si>
-    <t>Voltage dependent resistor</t>
-  </si>
-  <si>
     <t>Varistor</t>
   </si>
   <si>
@@ -725,9 +680,6 @@
     <t>Bourns Inc.</t>
   </si>
   <si>
-    <t>Two pin crystal</t>
-  </si>
-  <si>
     <t>Crystal</t>
   </si>
   <si>
@@ -776,10 +728,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-02-01 16:09:48</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.18 + KiBot v1.6.4</t>
+    <t>2024-03-27 09:47:42</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.18 + KiBot v1.6.5</t>
   </si>
   <si>
     <t>KiCad Fields (default)</t>
@@ -829,8 +781,6 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="$#,##0.00"/>
-    <numFmt numFmtId="164" formatCode="$#,##0.00"/>
     <numFmt numFmtId="164" formatCode="$#,##0.00"/>
   </numFmts>
   <fonts count="14">
@@ -960,7 +910,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE6F9FF"/>
+        <fgColor rgb="FFFF8080"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -972,19 +922,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8080"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF0FFF4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF0FFFF"/>
+        <fgColor rgb="FFFF8A8A"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -996,7 +940,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8A8A"/>
+        <fgColor rgb="FFE6F9FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0FFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1172,8 +1122,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1464384</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>16584</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -1224,8 +1174,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1464384</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>16584</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -1665,9 +1615,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="23.7109375" customWidth="1"/>
     <col min="6" max="6" width="46.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
@@ -1680,7 +1630,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1694,13 +1644,13 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="F2" s="3">
         <v>21</v>
@@ -1708,41 +1658,41 @@
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1750,13 +1700,13 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F6" s="3">
         <v>18</v>
@@ -1825,75 +1775,75 @@
       <c r="H9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="9" t="s">
+      <c r="B10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>21</v>
+      <c r="J10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="D11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>30</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>12</v>
@@ -1902,150 +1852,150 @@
         <v>19</v>
       </c>
       <c r="I11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="J11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" s="6" t="s">
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="D12" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="F12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>21</v>
+      <c r="J12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="A13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="G13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" s="6" t="s">
+      <c r="D14" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="E14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="10" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="9" t="s">
+      <c r="G14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="J14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="L14" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="11" t="s">
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="11" t="s">
+      <c r="B15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="11" t="s">
+      <c r="D15" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="J14" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K14" s="10" t="s">
+      <c r="E15" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="F15" s="7" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="45" customHeight="1">
-      <c r="A15" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>60</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>12</v>
@@ -2054,74 +2004,74 @@
         <v>19</v>
       </c>
       <c r="I15" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="E16" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="K15" s="6" t="s">
+      <c r="F16" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="G16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="30" customHeight="1">
-      <c r="A16" s="9" t="s">
+      <c r="B17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="D17" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="E17" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="F17" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K16" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L16" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="30" customHeight="1">
-      <c r="A17" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>12</v>
@@ -2129,75 +2079,75 @@
       <c r="H17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>21</v>
+      <c r="J17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18" s="9" t="s">
+      <c r="A18" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="12" t="s">
+      <c r="I18" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L18" s="12" t="s">
-        <v>21</v>
+      <c r="J18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="5" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>12</v>
@@ -2205,55 +2155,55 @@
       <c r="H19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" s="8" t="s">
-        <v>21</v>
+      <c r="J19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="G20" s="9" t="s">
+      <c r="A20" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="H20" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="12" t="s">
-        <v>21</v>
+      <c r="I20" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2278,9 +2228,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="44.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
@@ -2293,7 +2243,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2307,13 +2257,13 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="F2" s="3">
         <v>21</v>
@@ -2321,41 +2271,41 @@
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2363,13 +2313,13 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F6" s="3">
         <v>18</v>
@@ -2424,335 +2374,335 @@
         <v>14</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>17</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="I9" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="K9" s="8" t="s">
+      <c r="J9" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="G10" s="9" t="s">
+      <c r="B10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>21</v>
+      <c r="H10" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>122</v>
+        <v>13</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H11" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="L11" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="I11" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="J11" s="6" t="s">
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="L12" s="12" t="s">
         <v>121</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="45" customHeight="1">
-      <c r="A12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="K12" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="L12" s="10" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="45" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>135</v>
+        <v>13</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>141</v>
+        <v>125</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="I14" s="12" t="s">
+      <c r="A14" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>21</v>
+      <c r="J14" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="I15" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="K15" s="8" t="s">
+      <c r="J15" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="G16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="L16" s="10" t="s">
-        <v>149</v>
+      <c r="H16" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>153</v>
+        <v>13</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>160</v>
+        <v>142</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2782,14 +2732,14 @@
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="42.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="60.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2797,13 +2747,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -2811,13 +2761,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2826,13 +2776,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G21)</f>
@@ -2841,23 +2791,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2877,16 +2827,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2910,10 +2860,10 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>23</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>24</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>17</v>
@@ -2929,16 +2879,16 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="D12" s="19" t="s">
         <v>29</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>31</v>
       </c>
       <c r="E12" s="19">
         <f>BoardQty*1</f>
@@ -2951,13 +2901,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -2970,16 +2920,16 @@
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1">
       <c r="A14" s="19" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E14" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -2992,16 +2942,16 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="19" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E15" s="19">
         <f>BoardQty*1</f>
@@ -3014,16 +2964,16 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="19" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E16" s="19">
         <f>BoardQty*1</f>
@@ -3036,13 +2986,13 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="19" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E17" s="19">
         <f>BoardQty*1</f>
@@ -3055,13 +3005,13 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="19" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E18" s="19">
         <f>BoardQty*1</f>
@@ -3074,13 +3024,13 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="19" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E19" s="19">
         <f>CEILING(BoardQty*3,1)</f>
@@ -3093,13 +3043,13 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="19" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E20" s="19">
         <f>BoardQty*1</f>
@@ -3112,16 +3062,16 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="19" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="E21" s="19">
         <f>BoardQty*1</f>
@@ -3134,15 +3084,15 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="21" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="23" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -3240,14 +3190,14 @@
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="40.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="61.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3255,13 +3205,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3269,13 +3219,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3284,13 +3234,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G18)</f>
@@ -3299,23 +3249,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3335,24 +3285,24 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>17</v>
@@ -3368,16 +3318,16 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E11" s="19">
         <f>BoardQty*1</f>
@@ -3390,16 +3340,16 @@
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="E12" s="19">
         <f>BoardQty*1</f>
@@ -3412,16 +3362,16 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E13" s="19">
         <f>BoardQty*1</f>
@@ -3434,16 +3384,16 @@
     </row>
     <row r="14" spans="1:7" ht="45" customHeight="1">
       <c r="A14" s="19" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="E14" s="19">
         <f>BoardQty*1</f>
@@ -3456,13 +3406,13 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="19" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3475,13 +3425,13 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="19" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E16" s="19">
         <f>BoardQty*1</f>
@@ -3494,16 +3444,16 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="19" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="E17" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3516,16 +3466,16 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="19" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="E18" s="19">
         <f>BoardQty*1</f>
@@ -3538,15 +3488,15 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="21" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="23" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -3626,72 +3576,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="6" t="s">
-        <v>174</v>
+      <c r="A3" s="11" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="8" t="s">
-        <v>175</v>
+      <c r="A4" s="6" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ set-soft/kibot_variants_arduprog_test@f2b5671748de411d028c9745b59ca051d219371f 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/t1-bom.xlsx
+++ b/BoM/Costs/t1-bom.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="174">
   <si>
     <t>Row</t>
   </si>
@@ -476,6 +476,18 @@
     <t>10</t>
   </si>
   <si>
+    <t>Logo_Open_Hardware_Large</t>
+  </si>
+  <si>
+    <t>LOGO1</t>
+  </si>
+  <si>
+    <t>OSHW-Logo_11.4x12mm_SilkScreen</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>R</t>
   </si>
   <si>
@@ -488,7 +500,7 @@
     <t>R_0805_2012Metric</t>
   </si>
   <si>
-    <t>11</t>
+    <t>12</t>
   </si>
   <si>
     <t>R4</t>
@@ -497,7 +509,7 @@
     <t>10K</t>
   </si>
   <si>
-    <t>12</t>
+    <t>13</t>
   </si>
   <si>
     <t>ATmega8U2-A</t>
@@ -554,13 +566,13 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>30 (25 SMD/ 5 THT)</t>
+    <t>31 (25 SMD/ 5 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>18 (15 SMD/ 3 THT)</t>
+    <t>19 (15 SMD/ 3 THT)</t>
   </si>
   <si>
     <t>Number of PCBs:</t>
@@ -728,7 +740,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-04-10 14:28:37</t>
+    <t>2024-04-11 09:19:35</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.6</t>
@@ -1226,8 +1238,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>216609</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1531059</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
@@ -1605,7 +1617,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1616,9 +1628,9 @@
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
     <col min="6" max="6" width="46.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
@@ -1630,7 +1642,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1644,55 +1656,55 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F2" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1700,16 +1712,16 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F6" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2106,13 +2118,13 @@
         <v>71</v>
       </c>
       <c r="E18" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="10" t="s">
-        <v>73</v>
-      </c>
       <c r="G18" s="8" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>19</v>
@@ -2132,13 +2144,13 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>75</v>
@@ -2147,10 +2159,10 @@
         <v>76</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>19</v>
@@ -2170,13 +2182,13 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>79</v>
@@ -2185,7 +2197,7 @@
         <v>80</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>12</v>
@@ -2193,16 +2205,54 @@
       <c r="H20" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="J20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L20" s="9" t="s">
+      <c r="D21" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" s="6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2243,7 +2293,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2257,55 +2307,55 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F2" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2313,16 +2363,16 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F6" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2374,10 +2424,10 @@
         <v>14</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>17</v>
@@ -2386,13 +2436,13 @@
         <v>21</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>20</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="K9" s="6" t="s">
         <v>13</v>
@@ -2409,28 +2459,28 @@
         <v>13</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="K10" s="9" t="s">
         <v>13</v>
@@ -2447,34 +2497,34 @@
         <v>13</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="I11" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="J11" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="J11" s="11" t="s">
-        <v>110</v>
-      </c>
       <c r="K11" s="11" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -2485,34 +2535,34 @@
         <v>13</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>55</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>57</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="45" customHeight="1">
@@ -2523,34 +2573,34 @@
         <v>13</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -2561,28 +2611,28 @@
         <v>13</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>20</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="K14" s="9" t="s">
         <v>13</v>
@@ -2599,28 +2649,28 @@
         <v>13</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>20</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>13</v>
@@ -2637,34 +2687,34 @@
         <v>13</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="L16" s="12" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -2675,34 +2725,34 @@
         <v>13</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2717,7 +2767,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
@@ -2729,7 +2779,7 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="42.7109375" customWidth="1" outlineLevel="2"/>
     <col min="4" max="4" width="60.7109375" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="17.7109375" customWidth="1" outlineLevel="1"/>
@@ -2739,7 +2789,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2747,13 +2797,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -2761,13 +2811,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -2776,38 +2826,38 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="G4" s="16">
-        <f>SUM(G10:G21)</f>
+        <f>SUM(G10:G22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2827,16 +2877,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3027,14 +3077,14 @@
         <v>71</v>
       </c>
       <c r="B19" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="19" t="s">
-        <v>73</v>
-      </c>
       <c r="E19" s="19">
-        <f>CEILING(BoardQty*3,1)</f>
-        <v>3</v>
+        <f>BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="G19" s="20">
         <f>IF(AND(ISNUMBER(E19),ISNUMBER(F19)),E19*F19,"")</f>
@@ -3049,11 +3099,11 @@
         <v>76</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E20" s="19">
-        <f>BoardQty*1</f>
-        <v>1</v>
+        <f>CEILING(BoardQty*3,1)</f>
+        <v>3</v>
       </c>
       <c r="G20" s="20">
         <f>IF(AND(ISNUMBER(E20),ISNUMBER(F20)),E20*F20,"")</f>
@@ -3068,10 +3118,7 @@
         <v>80</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E21" s="19">
         <f>BoardQty*1</f>
@@ -3082,17 +3129,39 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>154</v>
+    <row r="22" spans="1:7">
+      <c r="A22" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="19">
+        <f>BoardQty*1</f>
+        <v>1</v>
+      </c>
+      <c r="G22" s="20">
+        <f>IF(AND(ISNUMBER(E22),ISNUMBER(F22)),E22*F22,"")</f>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="23" t="s">
-        <v>155</v>
+      <c r="A25" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="23" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3160,12 +3229,17 @@
       <formula>AND(ISBLANK(D21),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="expression" dxfId="0" priority="13">
+      <formula>AND(ISBLANK(D22),TRUE())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D12" r:id="rId1"/>
     <hyperlink ref="D14" r:id="rId2"/>
     <hyperlink ref="D15" r:id="rId3"/>
     <hyperlink ref="D16" r:id="rId4"/>
-    <hyperlink ref="D21" r:id="rId5"/>
+    <hyperlink ref="D22" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId6"/>
@@ -3197,7 +3271,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3205,13 +3279,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="D2" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="G2" s="13">
         <v>1</v>
@@ -3219,13 +3293,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="G3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3234,13 +3308,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="D4" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="G4" s="16">
         <f>SUM(G10:G18)</f>
@@ -3249,23 +3323,23 @@
     </row>
     <row r="5" spans="1:7">
       <c r="D5" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3285,24 +3359,24 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="19" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>17</v>
@@ -3318,16 +3392,16 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="19" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E11" s="19">
         <f>BoardQty*1</f>
@@ -3340,16 +3414,16 @@
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1">
       <c r="A12" s="19" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="E12" s="19">
         <f>BoardQty*1</f>
@@ -3362,13 +3436,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="19" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>55</v>
@@ -3384,16 +3458,16 @@
     </row>
     <row r="14" spans="1:7" ht="45" customHeight="1">
       <c r="A14" s="19" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E14" s="19">
         <f>BoardQty*1</f>
@@ -3406,13 +3480,13 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="19" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3425,13 +3499,13 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="19" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E16" s="19">
         <f>BoardQty*1</f>
@@ -3444,16 +3518,16 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="19" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E17" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3466,16 +3540,16 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="19" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="E18" s="19">
         <f>BoardQty*1</f>
@@ -3488,15 +3562,15 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="21" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="23" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3576,72 +3650,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="11" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="6" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ set-soft/kibot_variants_arduprog_test@3a250a0e673ff2005b39d0bb688751c13561674d 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/t1-bom.xlsx
+++ b/BoM/Costs/t1-bom.xlsx
@@ -14,12 +14,12 @@
     <sheet name="Colors" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="BoardQty" localSheetId="3">'Costs (DNF)'!$G$2</definedName>
-    <definedName name="BoardQty" localSheetId="2">'Costs'!$G$2</definedName>
+    <definedName name="BoardQty" localSheetId="3">'Costs (DNF)'!$H$2</definedName>
+    <definedName name="BoardQty" localSheetId="2">'Costs'!$H$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">BoM!$9:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">DNF!$9:$9</definedName>
-    <definedName name="TotalCost" localSheetId="3">'Costs (DNF)'!$G$4</definedName>
-    <definedName name="TotalCost" localSheetId="2">'Costs'!$G$4</definedName>
+    <definedName name="TotalCost" localSheetId="3">'Costs (DNF)'!$H$4</definedName>
+    <definedName name="TotalCost" localSheetId="2">'Costs'!$H$4</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -31,7 +31,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="F4" authorId="0">
+    <comment ref="G4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -79,11 +79,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Description of each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>PCB footprint for each part.</t>
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="0">
+    <comment ref="E9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0">
+    <comment ref="F9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -114,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0">
+    <comment ref="G9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0">
+    <comment ref="H9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -150,7 +163,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="F4" authorId="0">
+    <comment ref="G4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -198,11 +211,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Description of each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>PCB footprint for each part.</t>
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="0">
+    <comment ref="E9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -216,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0">
+    <comment ref="F9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -233,7 +259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0">
+    <comment ref="G9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -246,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0">
+    <comment ref="H9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -264,7 +290,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="195">
   <si>
     <t>Row</t>
   </si>
@@ -302,6 +328,24 @@
     <t>MFP</t>
   </si>
   <si>
+    <t>Sim.Name</t>
+  </si>
+  <si>
+    <t>Sim.Device</t>
+  </si>
+  <si>
+    <t>Sim.Pins</t>
+  </si>
+  <si>
+    <t>Sim.Params</t>
+  </si>
+  <si>
+    <t>Sim.Library</t>
+  </si>
+  <si>
+    <t>Sim.Enable</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -353,9 +397,6 @@
     <t>CP_Elec_8x10</t>
   </si>
   <si>
-    <t>https://www.vishay.com/docs/28388/153crv.pdf</t>
-  </si>
-  <si>
     <t>Vishay Beyschlag/Draloric/BC Components</t>
   </si>
   <si>
@@ -374,6 +415,9 @@
     <t>D_1206_3216Metric</t>
   </si>
   <si>
+    <t>1=K 2=A</t>
+  </si>
+  <si>
     <t>5</t>
   </si>
   <si>
@@ -386,9 +430,6 @@
     <t>LED_0805_2012Metric</t>
   </si>
   <si>
-    <t>https://dammedia.osram.info/media/resource/hires/osram-dam-2493936/LG%20R971.pdf</t>
-  </si>
-  <si>
     <t>OSRAM Opto Semiconductors Inc.</t>
   </si>
   <si>
@@ -407,9 +448,6 @@
     <t>BarrelJack_CLIFF_FC681465S_SMT_Horizontal</t>
   </si>
   <si>
-    <t>https://www.we-online.de/katalog/datasheet/6941xx106102.pdf</t>
-  </si>
-  <si>
     <t>Würth Elektronik</t>
   </si>
   <si>
@@ -431,9 +469,6 @@
     <t>PinHeader_2x03_P2.54mm_Vertical</t>
   </si>
   <si>
-    <t>https://cdn.harwin.com/pdfs/M20-998.pdf</t>
-  </si>
-  <si>
     <t>-USB</t>
   </si>
   <si>
@@ -446,7 +481,7 @@
     <t>8</t>
   </si>
   <si>
-    <t>Conn_01x05_Male</t>
+    <t>Conn_01x05_Pin</t>
   </si>
   <si>
     <t>J3</t>
@@ -461,7 +496,7 @@
     <t>9</t>
   </si>
   <si>
-    <t>Conn_01x06_Male</t>
+    <t>Conn_01x06_Pin</t>
   </si>
   <si>
     <t>J6</t>
@@ -485,6 +520,9 @@
     <t>OSHW-Logo_11.4x12mm_SilkScreen</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
     <t>11</t>
   </si>
   <si>
@@ -605,9 +643,6 @@
     <t>R_1812_4532Metric</t>
   </si>
   <si>
-    <t>https://www.bourns.com/docs/Product-Datasheets/mfmsmf.pdf</t>
-  </si>
-  <si>
     <t>+USB</t>
   </si>
   <si>
@@ -620,9 +655,6 @@
     <t>BLM21PG221SN1D</t>
   </si>
   <si>
-    <t>https://www.murata.com/en-eu/api/pdfdownloadapi?cate=cgsubChipFerriBead&amp;partno=BLM21PG221SN1%23</t>
-  </si>
-  <si>
     <t>Murata</t>
   </si>
   <si>
@@ -653,9 +685,6 @@
     <t>USB_B_Lumberg_2411_02_Horizontal</t>
   </si>
   <si>
-    <t>https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=292304&amp;DocType=Customer+Drawing&amp;DocLang=English</t>
-  </si>
-  <si>
     <t>TE Connectivity AMP Connectors</t>
   </si>
   <si>
@@ -686,12 +715,24 @@
     <t>R_0603_1608Metric</t>
   </si>
   <si>
-    <t>https://www.bourns.com/docs/Product-Datasheets/MLC.pdf</t>
-  </si>
-  <si>
     <t>Bourns Inc.</t>
   </si>
   <si>
+    <t>kicad_builtin_varistor</t>
+  </si>
+  <si>
+    <t>SUBCKT</t>
+  </si>
+  <si>
+    <t>1=A 2=B</t>
+  </si>
+  <si>
+    <t>threshold=1k</t>
+  </si>
+  <si>
+    <t>/usr/share/kicad/symbols/Simulation_SPICE.sp</t>
+  </si>
+  <si>
     <t>Crystal</t>
   </si>
   <si>
@@ -704,9 +745,6 @@
     <t>Crystal_SMD_Abracon_ABM3-2Pin_5.0x3.2mm</t>
   </si>
   <si>
-    <t>https://www.foxonline.com/pdfs/C4ST.pdf</t>
-  </si>
-  <si>
     <t>Abracon LLC</t>
   </si>
   <si>
@@ -728,6 +766,39 @@
     <t>Ext$</t>
   </si>
   <si>
+    <t>Unpolarized capacitor</t>
+  </si>
+  <si>
+    <t>Polarized capacitor</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>Light emitting diode</t>
+  </si>
+  <si>
+    <t>DC Barrel Jack with an internal switch</t>
+  </si>
+  <si>
+    <t>Generic connector, double row, 02x03, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x05, script generated</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x06, script generated</t>
+  </si>
+  <si>
+    <t>Open Hardware logo, large</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>16MHz, 8kB Flash, 512B SRAM, 512B EEPROM, TQFP-32</t>
+  </si>
+  <si>
     <t>Board Qty:</t>
   </si>
   <si>
@@ -740,10 +811,28 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-04-11 09:19:35</t>
+    <t>2024-04-11 10:40:33</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.6</t>
+  </si>
+  <si>
+    <t>Resettable fuse, polymeric positive temperature coefficient</t>
+  </si>
+  <si>
+    <t>Ferrite bead</t>
+  </si>
+  <si>
+    <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>USB Type B connector</t>
+  </si>
+  <si>
+    <t>Voltage dependent resistor</t>
+  </si>
+  <si>
+    <t>Two pin crystal</t>
   </si>
   <si>
     <t>KiCad Fields (default)</t>
@@ -1617,7 +1706,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1638,11 +1727,17 @@
     <col min="10" max="10" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="44.7109375" customWidth="1"/>
     <col min="12" max="12" width="19.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" customWidth="1"/>
+    <col min="17" max="17" width="21.7109375" customWidth="1"/>
+    <col min="18" max="18" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="32" customHeight="1">
+    <row r="1" spans="1:18" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1653,78 +1748,84 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+    </row>
+    <row r="2" spans="1:18">
       <c r="C2" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F2" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:18">
       <c r="C3" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="C4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="C5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="C4" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="C5" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:18">
       <c r="C6" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F6" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:18">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -1761,504 +1862,756 @@
       <c r="L8" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="H10" s="8" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>19</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R10" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="I12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="J12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R12" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K11" s="11" t="s">
+      <c r="H13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R14" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R16" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R17" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R18" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L11" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="8" t="s">
+      <c r="H19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R19" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L12" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="30" customHeight="1">
-      <c r="A13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L16" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L18" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="H20" s="8" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>19</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R20" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" s="5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R21" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:L1"/>
+    <mergeCell ref="C1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -2268,7 +2621,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -2285,15 +2638,21 @@
     <col min="6" max="6" width="44.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="60.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="35.7109375" customWidth="1"/>
     <col min="12" max="12" width="24.7109375" customWidth="1"/>
+    <col min="13" max="13" width="27.7109375" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" customWidth="1"/>
+    <col min="17" max="17" width="49.7109375" customWidth="1"/>
+    <col min="18" max="18" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="32" customHeight="1">
+    <row r="1" spans="1:18" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2304,78 +2663,84 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+    </row>
+    <row r="2" spans="1:18">
       <c r="C2" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F2" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:18">
       <c r="C3" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="C4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="C5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="C4" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="C5" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:18">
       <c r="C6" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F6" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:18">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -2412,352 +2777,532 @@
       <c r="L8" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>19</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="8" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E10" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="I10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R10" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R12" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R14" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="30" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E11" s="7" t="s">
+      <c r="K15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="12" t="s">
         <v>117</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="L11" s="11" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="45" customHeight="1">
-      <c r="A13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>114</v>
       </c>
       <c r="K16" s="12" t="s">
         <v>141</v>
       </c>
       <c r="L16" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>139</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="O16" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="P16" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q16" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="R16" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>146</v>
+        <v>111</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>148</v>
+        <v>152</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R17" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:L1"/>
+    <mergeCell ref="C1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -2767,11 +3312,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <pane xSplit="8" ySplit="9" topLeftCell="I10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -2780,84 +3325,86 @@
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="42.7109375" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="60.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="61.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="42.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="5" max="5" width="60.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32" customHeight="1">
+    <row r="1" spans="1:8" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="D2" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="G2" s="13">
+        <v>93</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="D3" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="G3" s="15">
+        <v>95</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
         <v>0.0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="D4" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="G4" s="16">
-        <f>SUM(G10:G22)</f>
+        <v>97</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="H4" s="16">
+        <f>SUM(H10:H22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="D5" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2865,8 +3412,9 @@
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="17"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="18" t="s">
         <v>3</v>
       </c>
@@ -2874,386 +3422,412 @@
         <v>4</v>
       </c>
       <c r="C9" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>150</v>
-      </c>
       <c r="E9" s="18" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>156</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="19" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="19">
+        <v>158</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="19">
         <f>CEILING(BoardQty*4,1)</f>
         <v>4</v>
       </c>
-      <c r="G10" s="20">
-        <f>IF(AND(ISNUMBER(E10),ISNUMBER(F10)),E10*F10,"")</f>
+      <c r="H10" s="20">
+        <f>IF(AND(ISNUMBER(F10),ISNUMBER(G10)),F10*G10,"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" s="19" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B11" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="19">
+      <c r="F11" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G11" s="20">
-        <f>IF(AND(ISNUMBER(E11),ISNUMBER(F11)),E11*F11,"")</f>
+      <c r="H11" s="20">
+        <f>IF(AND(ISNUMBER(F11),ISNUMBER(G11)),F11*G11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" s="19" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>28</v>
+        <v>159</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="19">
+        <v>34</v>
+      </c>
+      <c r="F12" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G12" s="20">
-        <f>IF(AND(ISNUMBER(E12),ISNUMBER(F12)),E12*F12,"")</f>
+      <c r="H12" s="20">
+        <f>IF(AND(ISNUMBER(F12),ISNUMBER(G12)),F12*G12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" s="19" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="19">
+        <v>160</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G13" s="20">
-        <f>IF(AND(ISNUMBER(E13),ISNUMBER(F13)),E13*F13,"")</f>
+      <c r="H13" s="20">
+        <f>IF(AND(ISNUMBER(F13),ISNUMBER(G13)),F13*G13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" customHeight="1">
+    <row r="14" spans="1:8">
       <c r="A14" s="19" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>39</v>
+        <v>161</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="19">
+        <v>45</v>
+      </c>
+      <c r="F14" s="19">
         <f>CEILING(BoardQty*2,1)</f>
         <v>2</v>
       </c>
-      <c r="G14" s="20">
-        <f>IF(AND(ISNUMBER(E14),ISNUMBER(F14)),E14*F14,"")</f>
+      <c r="H14" s="20">
+        <f>IF(AND(ISNUMBER(F14),ISNUMBER(G14)),F14*G14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" s="19" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>46</v>
+        <v>162</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="19">
+        <v>51</v>
+      </c>
+      <c r="F15" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G15" s="20">
-        <f>IF(AND(ISNUMBER(E15),ISNUMBER(F15)),E15*F15,"")</f>
+      <c r="H15" s="20">
+        <f>IF(AND(ISNUMBER(F15),ISNUMBER(G15)),F15*G15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8" ht="45" customHeight="1">
       <c r="A16" s="19" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>54</v>
+        <v>163</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="19">
+        <v>58</v>
+      </c>
+      <c r="F16" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G16" s="20">
-        <f>IF(AND(ISNUMBER(E16),ISNUMBER(F16)),E16*F16,"")</f>
+      <c r="H16" s="20">
+        <f>IF(AND(ISNUMBER(F16),ISNUMBER(G16)),F16*G16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17" s="19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="19">
+        <v>164</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G17" s="20">
-        <f>IF(AND(ISNUMBER(E17),ISNUMBER(F17)),E17*F17,"")</f>
+      <c r="H17" s="20">
+        <f>IF(AND(ISNUMBER(F17),ISNUMBER(G17)),F17*G17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18" s="19" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="19">
+        <v>165</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G18" s="20">
-        <f>IF(AND(ISNUMBER(E18),ISNUMBER(F18)),E18*F18,"")</f>
+      <c r="H18" s="20">
+        <f>IF(AND(ISNUMBER(F18),ISNUMBER(G18)),F18*G18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="A19" s="19" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" s="19">
+        <v>166</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G19" s="20">
-        <f>IF(AND(ISNUMBER(E19),ISNUMBER(F19)),E19*F19,"")</f>
+      <c r="H19" s="20">
+        <f>IF(AND(ISNUMBER(F19),ISNUMBER(G19)),F19*G19,"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8">
       <c r="A20" s="19" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="19">
+        <v>167</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="19">
         <f>CEILING(BoardQty*3,1)</f>
         <v>3</v>
       </c>
-      <c r="G20" s="20">
-        <f>IF(AND(ISNUMBER(E20),ISNUMBER(F20)),E20*F20,"")</f>
+      <c r="H20" s="20">
+        <f>IF(AND(ISNUMBER(F20),ISNUMBER(G20)),F20*G20,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8">
       <c r="A21" s="19" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" s="19">
+        <v>167</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G21" s="20">
-        <f>IF(AND(ISNUMBER(E21),ISNUMBER(F21)),E21*F21,"")</f>
+      <c r="H21" s="20">
+        <f>IF(AND(ISNUMBER(F21),ISNUMBER(G21)),F21*G21,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8">
       <c r="A22" s="19" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="E22" s="19">
+        <v>89</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G22" s="20">
-        <f>IF(AND(ISNUMBER(E22),ISNUMBER(F22)),E22*F22,"")</f>
+      <c r="H22" s="20">
+        <f>IF(AND(ISNUMBER(F22),ISNUMBER(G22)),F22*G22,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:8">
       <c r="A25" s="21" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="23" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="D1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E10">
+  <conditionalFormatting sqref="F10">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(ISBLANK(D10),TRUE())</formula>
+      <formula>AND(ISBLANK(E10),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
+  <conditionalFormatting sqref="F11">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>AND(ISBLANK(D11),TRUE())</formula>
+      <formula>AND(ISBLANK(E11),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
+  <conditionalFormatting sqref="F12">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>AND(ISBLANK(D12),TRUE())</formula>
+      <formula>AND(ISBLANK(E12),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
+  <conditionalFormatting sqref="F13">
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>AND(ISBLANK(D13),TRUE())</formula>
+      <formula>AND(ISBLANK(E13),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
+  <conditionalFormatting sqref="F14">
     <cfRule type="expression" dxfId="0" priority="5">
-      <formula>AND(ISBLANK(D14),TRUE())</formula>
+      <formula>AND(ISBLANK(E14),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15">
+  <conditionalFormatting sqref="F15">
     <cfRule type="expression" dxfId="0" priority="6">
-      <formula>AND(ISBLANK(D15),TRUE())</formula>
+      <formula>AND(ISBLANK(E15),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E16">
+  <conditionalFormatting sqref="F16">
     <cfRule type="expression" dxfId="0" priority="7">
-      <formula>AND(ISBLANK(D16),TRUE())</formula>
+      <formula>AND(ISBLANK(E16),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
+  <conditionalFormatting sqref="F17">
     <cfRule type="expression" dxfId="0" priority="8">
-      <formula>AND(ISBLANK(D17),TRUE())</formula>
+      <formula>AND(ISBLANK(E17),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
+  <conditionalFormatting sqref="F18">
     <cfRule type="expression" dxfId="0" priority="9">
-      <formula>AND(ISBLANK(D18),TRUE())</formula>
+      <formula>AND(ISBLANK(E18),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
+  <conditionalFormatting sqref="F19">
     <cfRule type="expression" dxfId="0" priority="10">
-      <formula>AND(ISBLANK(D19),TRUE())</formula>
+      <formula>AND(ISBLANK(E19),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E20">
+  <conditionalFormatting sqref="F20">
     <cfRule type="expression" dxfId="0" priority="11">
-      <formula>AND(ISBLANK(D20),TRUE())</formula>
+      <formula>AND(ISBLANK(E20),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
+  <conditionalFormatting sqref="F21">
     <cfRule type="expression" dxfId="0" priority="12">
-      <formula>AND(ISBLANK(D21),TRUE())</formula>
+      <formula>AND(ISBLANK(E21),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
+  <conditionalFormatting sqref="F22">
     <cfRule type="expression" dxfId="0" priority="13">
-      <formula>AND(ISBLANK(D22),TRUE())</formula>
+      <formula>AND(ISBLANK(E22),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D12" r:id="rId1"/>
-    <hyperlink ref="D14" r:id="rId2"/>
-    <hyperlink ref="D15" r:id="rId3"/>
-    <hyperlink ref="D16" r:id="rId4"/>
-    <hyperlink ref="D22" r:id="rId5"/>
+    <hyperlink ref="E22" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId6"/>
-  <legacyDrawing r:id="rId7"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="7" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <pane xSplit="8" ySplit="9" topLeftCell="I10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight"/>
     </sheetView>
@@ -3262,84 +3836,86 @@
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="4" width="61.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="61.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1" outlineLevel="2"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32" customHeight="1">
+    <row r="1" spans="1:8" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="D2" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="G2" s="13">
+        <v>93</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="D3" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="G3" s="15">
+        <v>95</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
         <v>0.0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="D4" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="G4" s="16">
-        <f>SUM(G10:G18)</f>
+        <v>97</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="H4" s="16">
+        <f>SUM(H10:H18)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="D5" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3347,8 +3923,9 @@
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="17"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="18" t="s">
         <v>3</v>
       </c>
@@ -3356,284 +3933,288 @@
         <v>4</v>
       </c>
       <c r="C9" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>150</v>
-      </c>
       <c r="E9" s="18" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>156</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="19" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="19">
+        <v>158</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
         <v>2</v>
       </c>
-      <c r="G10" s="20">
-        <f>IF(AND(ISNUMBER(E10),ISNUMBER(F10)),E10*F10,"")</f>
+      <c r="H10" s="20">
+        <f>IF(AND(ISNUMBER(F10),ISNUMBER(G10)),F10*G10,"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" s="19" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>112</v>
+        <v>175</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="E11" s="19">
+        <v>116</v>
+      </c>
+      <c r="F11" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G11" s="20">
-        <f>IF(AND(ISNUMBER(E11),ISNUMBER(F11)),E11*F11,"")</f>
+      <c r="H11" s="20">
+        <f>IF(AND(ISNUMBER(F11),ISNUMBER(G11)),F11*G11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" customHeight="1">
+    <row r="12" spans="1:8">
       <c r="A12" s="19" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>77</v>
+        <v>176</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="E12" s="19">
+        <v>81</v>
+      </c>
+      <c r="F12" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G12" s="20">
-        <f>IF(AND(ISNUMBER(E12),ISNUMBER(F12)),E12*F12,"")</f>
+      <c r="H12" s="20">
+        <f>IF(AND(ISNUMBER(F12),ISNUMBER(G12)),F12*G12,"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8" ht="45" customHeight="1">
       <c r="A13" s="19" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>123</v>
+        <v>177</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="19">
+        <v>125</v>
+      </c>
+      <c r="F13" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G13" s="20">
-        <f>IF(AND(ISNUMBER(E13),ISNUMBER(F13)),E13*F13,"")</f>
+      <c r="H13" s="20">
+        <f>IF(AND(ISNUMBER(F13),ISNUMBER(G13)),F13*G13,"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" customHeight="1">
+    <row r="14" spans="1:8">
       <c r="A14" s="19" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>128</v>
+        <v>178</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="E14" s="19">
+        <v>130</v>
+      </c>
+      <c r="F14" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G14" s="20">
-        <f>IF(AND(ISNUMBER(E14),ISNUMBER(F14)),E14*F14,"")</f>
+      <c r="H14" s="20">
+        <f>IF(AND(ISNUMBER(F14),ISNUMBER(G14)),F14*G14,"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" s="19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="E15" s="19">
+        <v>167</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
         <v>2</v>
       </c>
-      <c r="G15" s="20">
-        <f>IF(AND(ISNUMBER(E15),ISNUMBER(F15)),E15*F15,"")</f>
+      <c r="H15" s="20">
+        <f>IF(AND(ISNUMBER(F15),ISNUMBER(G15)),F15*G15,"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="19">
+        <v>167</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G16" s="20">
-        <f>IF(AND(ISNUMBER(E16),ISNUMBER(F16)),E16*F16,"")</f>
+      <c r="H16" s="20">
+        <f>IF(AND(ISNUMBER(F16),ISNUMBER(G16)),F16*G16,"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17" s="19" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>139</v>
+        <v>179</v>
       </c>
       <c r="D17" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="E17" s="19">
+      <c r="F17" s="19">
         <f>CEILING(BoardQty*2,1)</f>
         <v>2</v>
       </c>
-      <c r="G17" s="20">
-        <f>IF(AND(ISNUMBER(E17),ISNUMBER(F17)),E17*F17,"")</f>
+      <c r="H17" s="20">
+        <f>IF(AND(ISNUMBER(F17),ISNUMBER(G17)),F17*G17,"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18" s="19" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>145</v>
+        <v>180</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="E18" s="19">
+        <v>150</v>
+      </c>
+      <c r="F18" s="19">
         <f>BoardQty*1</f>
         <v>1</v>
       </c>
-      <c r="G18" s="20">
-        <f>IF(AND(ISNUMBER(E18),ISNUMBER(F18)),E18*F18,"")</f>
+      <c r="H18" s="20">
+        <f>IF(AND(ISNUMBER(F18),ISNUMBER(G18)),F18*G18,"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8">
       <c r="A21" s="21" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="23" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="D1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E10">
+  <conditionalFormatting sqref="F10">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(ISBLANK(D10),TRUE())</formula>
+      <formula>AND(ISBLANK(E10),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
+  <conditionalFormatting sqref="F11">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>AND(ISBLANK(D11),TRUE())</formula>
+      <formula>AND(ISBLANK(E11),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
+  <conditionalFormatting sqref="F12">
     <cfRule type="expression" dxfId="0" priority="3">
-      <formula>AND(ISBLANK(D12),TRUE())</formula>
+      <formula>AND(ISBLANK(E12),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
+  <conditionalFormatting sqref="F13">
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>AND(ISBLANK(D13),TRUE())</formula>
+      <formula>AND(ISBLANK(E13),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
+  <conditionalFormatting sqref="F14">
     <cfRule type="expression" dxfId="0" priority="5">
-      <formula>AND(ISBLANK(D14),TRUE())</formula>
+      <formula>AND(ISBLANK(E14),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15">
+  <conditionalFormatting sqref="F15">
     <cfRule type="expression" dxfId="0" priority="6">
-      <formula>AND(ISBLANK(D15),TRUE())</formula>
+      <formula>AND(ISBLANK(E15),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E16">
+  <conditionalFormatting sqref="F16">
     <cfRule type="expression" dxfId="0" priority="7">
-      <formula>AND(ISBLANK(D16),TRUE())</formula>
+      <formula>AND(ISBLANK(E16),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
+  <conditionalFormatting sqref="F17">
     <cfRule type="expression" dxfId="0" priority="8">
-      <formula>AND(ISBLANK(D17),TRUE())</formula>
+      <formula>AND(ISBLANK(E17),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
+  <conditionalFormatting sqref="F18">
     <cfRule type="expression" dxfId="0" priority="9">
-      <formula>AND(ISBLANK(D18),TRUE())</formula>
+      <formula>AND(ISBLANK(E18),TRUE())</formula>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1"/>
-    <hyperlink ref="D12" r:id="rId2"/>
-    <hyperlink ref="D13" r:id="rId3"/>
-    <hyperlink ref="D14" r:id="rId4"/>
-    <hyperlink ref="D17" r:id="rId5"/>
-    <hyperlink ref="D18" r:id="rId6"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId7"/>
-  <legacyDrawing r:id="rId8"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3650,72 +4231,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="11" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="6" t="s">
-        <v>163</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>173</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ set-soft/kibot_variants_arduprog_test@4207192516805dadb061ab48ca7460e92089fa0e 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/t1-bom.xlsx
+++ b/BoM/Costs/t1-bom.xlsx
@@ -290,7 +290,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="193">
   <si>
     <t>Row</t>
   </si>
@@ -343,9 +343,6 @@
     <t>Sim.Library</t>
   </si>
   <si>
-    <t>Sim.Enable</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -520,9 +517,6 @@
     <t>OSHW-Logo_11.4x12mm_SilkScreen</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
@@ -811,7 +805,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-04-11 11:58:11</t>
+    <t>2024-04-11 12:14:17</t>
   </si>
   <si>
     <t>KiCost® v1.1.18 + KiBot v1.6.6</t>
@@ -1706,7 +1700,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1732,12 +1726,11 @@
     <col min="15" max="15" width="18.7109375" customWidth="1"/>
     <col min="16" max="16" width="20.7109375" customWidth="1"/>
     <col min="17" max="17" width="21.7109375" customWidth="1"/>
-    <col min="18" max="18" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="32" customHeight="1">
+    <row r="1" spans="1:17" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1753,79 +1746,78 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-    </row>
-    <row r="2" spans="1:18">
+    </row>
+    <row r="2" spans="1:17">
       <c r="C2" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F2" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:17">
       <c r="C3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="C4" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
-      <c r="C4" s="2" t="s">
+    <row r="5" spans="1:17">
+      <c r="C5" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="C5" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:17">
       <c r="C6" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F6" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:17">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -1877,741 +1869,699 @@
       <c r="Q8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R8" s="4" t="s">
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="A9" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="B9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="J9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="B10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R9" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
-      <c r="A10" s="8" t="s">
+      <c r="D10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="8" t="s">
+      <c r="B12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="J12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="N10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="O10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="R10" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
-      <c r="A11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="5" t="s">
+      <c r="H13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="L11" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R11" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="A12" s="8" t="s">
+      <c r="J13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="8" t="s">
+      <c r="I14" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="N12" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="P12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="R12" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
-      <c r="A13" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="5" t="s">
+      <c r="J14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R13" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="A14" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="8" t="s">
+      <c r="J15" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="M14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="N14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="O14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="R14" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="A15" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="5" t="s">
+      <c r="J16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="P16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q16" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R15" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
-      <c r="A16" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="8" t="s">
+      <c r="J17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L16" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M16" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="N16" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="O16" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P16" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q16" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="R16" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18">
-      <c r="A17" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="5" t="s">
+      <c r="J18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="P18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q18" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R17" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18">
-      <c r="A18" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="8" t="s">
+      <c r="J19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q19" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="N18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="O18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="R18" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18">
-      <c r="A19" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R19" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18">
-      <c r="A20" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="10" t="s">
+      <c r="J20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="P20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q20" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="B21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F20" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L20" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M20" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="N20" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="O20" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P20" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q20" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="R20" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18">
-      <c r="A21" s="5" t="s">
+      <c r="D21" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="G21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F21" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>90</v>
-      </c>
       <c r="J21" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N21" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O21" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P21" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q21" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R21" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:R1"/>
+    <mergeCell ref="C1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -2621,7 +2571,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -2647,12 +2597,11 @@
     <col min="15" max="15" width="18.7109375" customWidth="1"/>
     <col min="16" max="16" width="20.7109375" customWidth="1"/>
     <col min="17" max="17" width="49.7109375" customWidth="1"/>
-    <col min="18" max="18" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="32" customHeight="1">
+    <row r="1" spans="1:17" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2668,79 +2617,78 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-    </row>
-    <row r="2" spans="1:18">
+    </row>
+    <row r="2" spans="1:17">
       <c r="C2" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F2" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:17">
       <c r="C3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="C4" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
-      <c r="C4" s="2" t="s">
+    <row r="5" spans="1:17">
+      <c r="C5" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="C5" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:17">
       <c r="C6" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F6" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:17">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -2792,517 +2740,487 @@
       <c r="Q8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R8" s="4" t="s">
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="A9" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="B9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>20</v>
-      </c>
       <c r="D9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="I9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="K9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="I9" s="6" t="s">
+      <c r="B12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R9" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
-      <c r="A10" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="E10" s="10" t="s">
+      <c r="H14" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="I10" s="9" t="s">
+      <c r="K14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="G16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="N10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="O10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="R10" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
-      <c r="A11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="L11" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R11" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="A12" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="N12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="O12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="R12" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
-      <c r="A13" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R13" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="A14" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="N14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="O14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="P14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="R14" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="A15" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R15" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
-      <c r="A16" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="H16" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="L16" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F16" s="10" t="s">
+      <c r="M16" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="G16" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="K16" s="12" t="s">
+      <c r="N16" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="L16" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="M16" s="12" t="s">
+      <c r="O16" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="N16" s="12" t="s">
+      <c r="P16" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="O16" s="12" t="s">
+      <c r="Q16" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="P16" s="12" t="s">
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="Q16" s="12" t="s">
+      <c r="D17" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="R16" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18">
-      <c r="A17" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="E17" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="G17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="K17" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="L17" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="L17" s="11" t="s">
-        <v>152</v>
-      </c>
       <c r="M17" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O17" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P17" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R17" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:R1"/>
+    <mergeCell ref="C1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -3335,7 +3253,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3344,13 +3262,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="D2" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H2" s="13">
         <v>1</v>
@@ -3358,13 +3276,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="D3" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3373,13 +3291,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="D4" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H4" s="16">
         <f>SUM(H10:H22)</f>
@@ -3388,23 +3306,23 @@
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3428,30 +3346,30 @@
         <v>5</v>
       </c>
       <c r="E9" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="H9" s="18" t="s">
         <v>155</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="C10" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>23</v>
       </c>
       <c r="F10" s="19">
         <f>CEILING(BoardQty*4,1)</f>
@@ -3464,16 +3382,16 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>29</v>
-      </c>
       <c r="C11" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" s="19">
         <f>BoardQty*1</f>
@@ -3486,16 +3404,16 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="C12" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="19" t="s">
         <v>33</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>34</v>
       </c>
       <c r="F12" s="19">
         <f>BoardQty*1</f>
@@ -3508,16 +3426,16 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="C13" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="D13" s="19" t="s">
         <v>39</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>40</v>
       </c>
       <c r="F13" s="19">
         <f>BoardQty*1</f>
@@ -3530,16 +3448,16 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="D14" s="19" t="s">
         <v>44</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>45</v>
       </c>
       <c r="F14" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3552,16 +3470,16 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>50</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>51</v>
       </c>
       <c r="F15" s="19">
         <f>BoardQty*1</f>
@@ -3574,16 +3492,16 @@
     </row>
     <row r="16" spans="1:8" ht="45" customHeight="1">
       <c r="A16" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="C16" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="D16" s="19" t="s">
         <v>57</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>58</v>
       </c>
       <c r="F16" s="19">
         <f>BoardQty*1</f>
@@ -3596,16 +3514,16 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="C17" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" s="19" t="s">
         <v>65</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>66</v>
       </c>
       <c r="F17" s="19">
         <f>BoardQty*1</f>
@@ -3618,16 +3536,16 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="C18" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D18" s="19" t="s">
         <v>70</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>71</v>
       </c>
       <c r="F18" s="19">
         <f>BoardQty*1</f>
@@ -3640,16 +3558,16 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="D19" s="19" t="s">
         <v>74</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>75</v>
       </c>
       <c r="F19" s="19">
         <f>BoardQty*1</f>
@@ -3662,16 +3580,16 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" s="19" t="s">
         <v>79</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>81</v>
       </c>
       <c r="F20" s="19">
         <f>CEILING(BoardQty*3,1)</f>
@@ -3684,16 +3602,16 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F21" s="19">
         <f>BoardQty*1</f>
@@ -3706,19 +3624,19 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D22" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="E22" s="19" t="s">
         <v>88</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>90</v>
       </c>
       <c r="F22" s="19">
         <f>BoardQty*1</f>
@@ -3731,15 +3649,15 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -3846,7 +3764,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="32" customHeight="1">
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3855,13 +3773,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="D2" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H2" s="13">
         <v>1</v>
@@ -3869,13 +3787,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="D3" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H3" s="15">
         <f>TotalCost/BoardQty</f>
@@ -3884,13 +3802,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="D4" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H4" s="16">
         <f>SUM(H10:H18)</f>
@@ -3899,23 +3817,23 @@
     </row>
     <row r="5" spans="1:8">
       <c r="D5" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="D6" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3939,30 +3857,30 @@
         <v>5</v>
       </c>
       <c r="E9" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="H9" s="18" t="s">
         <v>155</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -3975,16 +3893,16 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11" s="19" t="s">
         <v>114</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>116</v>
       </c>
       <c r="F11" s="19">
         <f>BoardQty*1</f>
@@ -3997,16 +3915,16 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F12" s="19">
         <f>BoardQty*1</f>
@@ -4019,16 +3937,16 @@
     </row>
     <row r="13" spans="1:8" ht="45" customHeight="1">
       <c r="A13" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="D13" s="19" t="s">
         <v>123</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>125</v>
       </c>
       <c r="F13" s="19">
         <f>BoardQty*1</f>
@@ -4041,16 +3959,16 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="19" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B14" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="D14" s="19" t="s">
         <v>128</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>130</v>
       </c>
       <c r="F14" s="19">
         <f>BoardQty*1</f>
@@ -4063,16 +3981,16 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F15" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4085,16 +4003,16 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F16" s="19">
         <f>BoardQty*1</f>
@@ -4107,16 +4025,16 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="D17" s="19" t="s">
         <v>138</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>140</v>
       </c>
       <c r="F17" s="19">
         <f>CEILING(BoardQty*2,1)</f>
@@ -4129,16 +4047,16 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="D18" s="19" t="s">
         <v>148</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>150</v>
       </c>
       <c r="F18" s="19">
         <f>BoardQty*1</f>
@@ -4151,15 +4069,15 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -4231,72 +4149,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="24" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="27" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="28" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="29" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="30" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="32" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ set-soft/kibot_variants_arduprog_test@bf25357590623ee6f2a543989aed2a4b3913eb00 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/t1-bom.xlsx
+++ b/BoM/Costs/t1-bom.xlsx
@@ -589,7 +589,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>8.0.4+1</t>
+    <t>8.0.5+1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -805,10 +805,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-09-25 11:41:32</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.19 + KiBot v1.8.1</t>
+    <t>2024-10-28 12:46:48</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.19 + KiBot v1.8.2</t>
   </si>
   <si>
     <t>Resettable fuse, polymeric positive temperature coefficient</t>
@@ -1222,10 +1222,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>16584</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123779</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1691100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>107315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1252,7 +1252,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2378784" cy="1285829"/>
+          <a:ext cx="9396825" cy="5079365"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1274,10 +1274,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>16584</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123779</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2691225</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>107315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1304,7 +1304,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2378784" cy="1285829"/>
+          <a:ext cx="9396825" cy="5079365"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1326,10 +1326,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1531059</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123779</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2719800</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>107315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1356,7 +1356,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2378784" cy="1285829"/>
+          <a:ext cx="9396825" cy="5079365"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1378,10 +1378,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>483309</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123779</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>671925</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>107315</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1408,7 +1408,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="2378784" cy="1285829"/>
+          <a:ext cx="9396825" cy="5079365"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>

<commit_message>
Deploying to main from @ set-soft/kibot_variants_arduprog_test@1e1f73bc0b1e218d2ab85a3f36532a25ee384d8b 🚀
</commit_message>
<xml_diff>
--- a/BoM/Costs/t1-bom.xlsx
+++ b/BoM/Costs/t1-bom.xlsx
@@ -589,7 +589,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>8.0.5+1</t>
+    <t>9.0.0</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -805,10 +805,10 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2024-10-29 10:47:52</t>
-  </si>
-  <si>
-    <t>KiCost® v1.1.19 + KiBot v1.8.2</t>
+    <t>2025-03-05 13:55:01</t>
+  </si>
+  <si>
+    <t>KiCost® v1.1.19 + KiBot v1.8.3</t>
   </si>
   <si>
     <t>Resettable fuse, polymeric positive temperature coefficient</t>
@@ -1222,10 +1222,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1691100</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>107315</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>16584</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1252,7 +1252,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9396825" cy="5079365"/>
+          <a:ext cx="2378784" cy="1285829"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1274,10 +1274,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2691225</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>107315</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>16584</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1304,7 +1304,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9396825" cy="5079365"/>
+          <a:ext cx="2378784" cy="1285829"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1326,10 +1326,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2719800</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>107315</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1531059</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1356,7 +1356,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9396825" cy="5079365"/>
+          <a:ext cx="2378784" cy="1285829"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1378,10 +1378,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>671925</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>107315</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>483309</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123779</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1408,7 +1408,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9396825" cy="5079365"/>
+          <a:ext cx="2378784" cy="1285829"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>